<commit_message>
Fixed bug with institution list
</commit_message>
<xml_diff>
--- a/test/HWDBUploader/SystemTest/Upload_PID.xlsx
+++ b/test/HWDBUploader/SystemTest/Upload_PID.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
   <si>
     <t xml:space="preserve">External ID</t>
   </si>
@@ -48,84 +48,87 @@
     <t xml:space="preserve">Flavor</t>
   </si>
   <si>
-    <t xml:space="preserve">Z00100300023-00074</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4A2B9EA4-D01D-45F2-8449-601BA6356EEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">generated 2023-10-12 07:36:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orange</t>
+    <t xml:space="preserve">Z00100300023-00082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3BE35F2B-E261-4DD5-BBF2-0FF6FE330BFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generated 2023-10-12 09:14:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strawberry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z00100300023-00083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1116BE19-0257-4F43-AA4E-D4ECD52D2E4E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z00100300023-00084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6252B910-67E0-4D50-8C57-DEFDD18AC09C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Violet</t>
   </si>
   <si>
     <t xml:space="preserve">Raspberry</t>
   </si>
   <si>
-    <t xml:space="preserve">Z00100300023-00075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1A8AB068-4066-4D08-82DC-FB97DB6EF542</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maroon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Butterscotch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z00100300023-00076</t>
-  </si>
-  <si>
-    <t xml:space="preserve">368A284E-39F0-4FE1-80CB-300C40098B5D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Almond</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z00100300023-00077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42CA3348-6FAE-45D8-979C-BFA617EB2E6A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coffee</t>
+    <t xml:space="preserve">Z00100300023-00085</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63E9366A-0320-42C7-9C3B-996F655B9298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow</t>
   </si>
   <si>
     <t xml:space="preserve">Image File</t>
   </si>
   <si>
-    <t xml:space="preserve">../images/banana.jpeg</t>
+    <t xml:space="preserve">../images/laughingcat.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../iamges/apple.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../images/raccoon.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../images/lightbulb.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../images/broccoli.jpeg</t>
   </si>
   <si>
     <t xml:space="preserve">../images/dice.jpeg</t>
   </si>
   <si>
-    <t xml:space="preserve">../images/lightbulb.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../iamges/apple.jpeg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Length</t>
   </si>
   <si>
@@ -141,16 +144,16 @@
     <t xml:space="preserve">Right Bongo</t>
   </si>
   <si>
-    <t xml:space="preserve">Z00100300022-00042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1330922A-8BFD-4B41-B5D4-96341A254CEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z00100300022-00043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77878EF9-D0EB-4430-ABB0-F667952D4ACF</t>
+    <t xml:space="preserve">Z00100300022-00046</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5D330D27-AA7C-46E6-A90F-ABE6980437D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z00100300022-00047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30A495F0-3094-4D66-B131-57715A15ECEB</t>
   </si>
   <si>
     <t xml:space="preserve">Result</t>
@@ -278,7 +281,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.75"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -392,7 +399,7 @@
         <v>22</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -417,7 +424,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -430,7 +437,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +451,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -458,7 +465,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,7 +479,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -486,7 +493,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +518,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -541,7 +548,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>30</v>
@@ -558,10 +565,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>31</v>
@@ -592,10 +599,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -620,7 +627,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -633,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +668,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +696,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -711,13 +718,13 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,27 +744,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>186</v>
@@ -769,27 +776,27 @@
         <v>9</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>109.44</v>
+        <v>81.34</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>113.29</v>
+        <v>81.64</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>82.82</v>
+        <v>83.84</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>186</v>
@@ -801,13 +808,13 @@
         <v>9</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>87.25</v>
+        <v>86.03</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>109.21</v>
+        <v>106.24</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>83.96</v>
+        <v>84.53</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>16</v>
@@ -838,7 +845,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -854,7 +861,7 @@
         <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>29</v>
@@ -862,39 +869,39 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>31</v>

</xml_diff>